<commit_message>
Changed novaseq x smallest container name in the template choices.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
@@ -348,7 +348,7 @@
     <t xml:space="preserve">illumina-novaseq-sp flowcell</t>
   </si>
   <si>
-    <t xml:space="preserve">illumina-novaseq-x-1_5b flowcell</t>
+    <t xml:space="preserve">illumina-novaseq-x-1.5b flowcell</t>
   </si>
   <si>
     <t xml:space="preserve">illumina-miseq-v2 flowcell</t>
@@ -9032,7 +9032,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.68"/>
   </cols>

</xml_diff>

<commit_message>
add serial number to instruments
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" state="visible" r:id="rId3"/>
@@ -359,7 +359,7 @@
     <t xml:space="preserve">Sample failed - Remove sample from study workflow</t>
   </si>
   <si>
-    <t xml:space="preserve">Carrie Derick</t>
+    <t xml:space="preserve">A01371R-Carrie Derick</t>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-s1 flowcell</t>
@@ -380,7 +380,7 @@
     <t xml:space="preserve">Repeat step - Move to next step and repeat current step</t>
   </si>
   <si>
-    <t xml:space="preserve">Barbara McClintock</t>
+    <t xml:space="preserve">A01861-Barbara McClintock</t>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-s2 flowcell</t>
@@ -398,7 +398,7 @@
     <t xml:space="preserve">Ignore workflow - Do not register as part of a workflow</t>
   </si>
   <si>
-    <t xml:space="preserve">Mykonos</t>
+    <t xml:space="preserve">M03555-Mykonos</t>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-s4 flowcell</t>
@@ -410,7 +410,7 @@
     <t xml:space="preserve">A05</t>
   </si>
   <si>
-    <t xml:space="preserve">Maurice</t>
+    <t xml:space="preserve">FS10000133-Maurice</t>
   </si>
   <si>
     <t xml:space="preserve">A06</t>
@@ -2069,7 +2069,7 @@
   </sheetPr>
   <dimension ref="A1:N996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -9411,7 +9411,7 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
move serial id into parenthesis
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
@@ -338,7 +338,25 @@
     <t xml:space="preserve">Step complete - Move to next step</t>
   </si>
   <si>
-    <t xml:space="preserve">LH00375-Rosalind Franklin</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rosalind Franklin (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">LH00375)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-sp flowcell</t>
@@ -362,7 +380,25 @@
     <t xml:space="preserve">Sample failed - Remove sample from study workflow</t>
   </si>
   <si>
-    <t xml:space="preserve">A01371R-Carrie Derick</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Carrie Derick (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">A01371R)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-s1 flowcell</t>
@@ -383,7 +419,25 @@
     <t xml:space="preserve">Repeat step - Move to next step and repeat current step</t>
   </si>
   <si>
-    <t xml:space="preserve">A01861-Barbara McClintock</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Barbara McClintock (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">A01861)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-s2 flowcell</t>
@@ -401,7 +455,25 @@
     <t xml:space="preserve">Ignore workflow - Do not register as part of a workflow</t>
   </si>
   <si>
-    <t xml:space="preserve">M03555-Mykonos</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mykonos (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">M03555)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-s4 flowcell</t>
@@ -413,7 +485,25 @@
     <t xml:space="preserve">A05</t>
   </si>
   <si>
-    <t xml:space="preserve">FS10000133-Maurice</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Maurice (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">FS10000133)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">A06</t>
@@ -1562,7 +1652,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1671,6 +1761,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="6">
@@ -9504,7 +9600,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -9539,7 +9635,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>82</v>
       </c>
@@ -9571,7 +9667,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
@@ -9603,7 +9699,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>96</v>
       </c>
@@ -9629,7 +9725,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
increase instrument column width
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Experiments" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Samples" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Info" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Index" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Experiments" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Samples" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Info" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Index" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="iSeq_flowcells" vbProcedure="false">Index!$K$2</definedName>
@@ -31,16 +31,18 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Illumina Flowcell Barcode</t>
         </r>
@@ -53,16 +55,18 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="G4" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">A01: Lane 1
 A02: Lane 2
@@ -338,25 +342,7 @@
     <t xml:space="preserve">Step complete - Move to next step</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Rosalind Franklin (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">LH00375)</t>
-    </r>
+    <t xml:space="preserve">Rosalind Franklin (LH00375)</t>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-sp flowcell</t>
@@ -380,25 +366,7 @@
     <t xml:space="preserve">Sample failed - Remove sample from study workflow</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Carrie Derick (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">A01371R)</t>
-    </r>
+    <t xml:space="preserve">Carrie Derick (A01371R)</t>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-s1 flowcell</t>
@@ -419,25 +387,7 @@
     <t xml:space="preserve">Repeat step - Move to next step and repeat current step</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Barbara McClintock (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">A01861)</t>
-    </r>
+    <t xml:space="preserve">Barbara McClintock (A01861)</t>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-s2 flowcell</t>
@@ -455,25 +405,7 @@
     <t xml:space="preserve">Ignore workflow - Do not register as part of a workflow</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mykonos (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">M03555)</t>
-    </r>
+    <t xml:space="preserve">Mykonos (M03555)</t>
   </si>
   <si>
     <t xml:space="preserve">illumina-novaseq-s4 flowcell</t>
@@ -485,25 +417,7 @@
     <t xml:space="preserve">A05</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Maurice (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">FS10000133)</t>
-    </r>
+    <t xml:space="preserve">Maurice (FS10000133)</t>
   </si>
   <si>
     <t xml:space="preserve">A06</t>
@@ -1652,7 +1566,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1713,11 +1627,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="13"/>
       <color rgb="FF000000"/>
@@ -1761,12 +1670,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1947,11 +1850,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1963,27 +1870,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2059,114 +1962,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4844,7 +4641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9229,7 +9026,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9539,7 +9336,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9556,7 +9353,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.21"/>

</xml_diff>

<commit_message>
Replaced N/A that gets parsed to a null value to No Side.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
@@ -31,7 +31,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>UFG</author>
   </authors>
   <commentList>
     <comment ref="B6" authorId="0">
@@ -55,7 +55,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>UFG</author>
   </authors>
   <commentList>
     <comment ref="G4" authorId="0">
@@ -381,7 +381,7 @@
     <t xml:space="preserve">A03</t>
   </si>
   <si>
-    <t xml:space="preserve">N/A</t>
+    <t xml:space="preserve">No Side</t>
   </si>
   <si>
     <t xml:space="preserve">Repeat step - Move to next step and repeat current step</t>
@@ -4616,22 +4616,22 @@
     <mergeCell ref="G5:H5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L7:L27" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L7:L27" type="list">
       <formula1>Index!$D$2:$D$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C7:C100" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C7:C100" type="list">
       <formula1>Index!$F$2:$F$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D7:D100" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D7:D100" type="list">
       <formula1>INDIRECT(SUBSTITUTE(INDEX(Index!$G$2:$G$6, MATCH(C7, Index!$F$2:$F$6, 0), 1), " ", "_"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8993,30 +8993,30 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D101" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D101" type="list">
       <formula1>Index!$B$2:$B$97</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
       <formula1>Experiments!$A$7:$A$106</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5:I100" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5:I100" type="list">
       <formula1>Index!$E$2:$E$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E5:E101" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E5:E101" type="none">
       <formula1>Index!$B$2:$B$97</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G5:G1000" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G5:G1000" type="list">
       <formula1>"1,2,3,4,5,6,7,8,A01,A02,A03,A04,A05,A06,A07,A08"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -9327,7 +9327,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -12334,7 +12334,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Apply sequencer side dropdown up to row 100.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_illumina_v4_8_0.xlsx
@@ -2159,7 +2159,7 @@
       <c r="F7" s="14"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2167,7 +2167,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2175,7 +2175,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2183,7 +2183,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2191,7 +2191,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2199,7 +2199,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2207,7 +2207,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2215,7 +2215,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2223,7 +2223,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -4616,7 +4616,7 @@
     <mergeCell ref="G5:H5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L7:L27" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L7:L100" type="list">
       <formula1>Index!$D$2:$D$4</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>